<commit_message>
Extent Report Enhancement part2
</commit_message>
<xml_diff>
--- a/src/main/java/resources/StudentDetails.xlsx
+++ b/src/main/java/resources/StudentDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="8">
   <si>
     <t>Sn</t>
   </si>
@@ -705,7 +705,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -738,6 +738,8 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="true"/>
@@ -1139,7 +1141,7 @@
       <c r="C2" s="4">
         <v>8789998079</v>
       </c>
-      <c r="D2" t="s" s="62">
+      <c r="D2" t="s" s="64">
         <v>7</v>
       </c>
     </row>
@@ -1153,7 +1155,7 @@
       <c r="C3" s="4">
         <v>9576675761</v>
       </c>
-      <c r="D3" t="s" s="63">
+      <c r="D3" t="s" s="65">
         <v>7</v>
       </c>
     </row>

</xml_diff>